<commit_message>
Zmieniono wygląd MainPage. Dodano Kafelki Opisujące statystyki konta zamast zwykłych label z tekstem
</commit_message>
<xml_diff>
--- a/MauiApp1.Test/Plik_xtb_do_testow.xlsx
+++ b/MauiApp1.Test/Plik_xtb_do_testow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\Documents\Visual Studio 2022\Portfolio-Tracker\MauiApp1.Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F3E3FD-654C-4E65-9C02-810DE3911547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745EC3BB-C216-443D-AF78-EAC8381A41C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="4215" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D0F3F6B9-96A1-438E-B47A-37E3DCA5E30A}"/>
+    <workbookView xWindow="2010" yWindow="3330" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{D0F3F6B9-96A1-438E-B47A-37E3DCA5E30A}"/>
   </bookViews>
   <sheets>
     <sheet name="CLOSED POSITION HISTORY" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="78">
   <si>
     <t/>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>odesetki</t>
+  </si>
+  <si>
+    <t>dywidenda pko</t>
   </si>
 </sst>
 </file>
@@ -2093,7 +2096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCA9AD0-EF6B-43F0-B05E-5472A2BEDAD1}">
   <dimension ref="B7:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -2585,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3074FF5-456E-48C8-B2D2-F37D01749490}">
-  <dimension ref="B12:L27"/>
+  <dimension ref="B12:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,7 +2713,7 @@
         <v>-3000</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>5</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <v>6</v>
       </c>
@@ -2749,8 +2752,15 @@
       <c r="G18" s="29">
         <v>-47.5</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M18" s="54">
+        <f>G17+G18</f>
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>7</v>
       </c>
@@ -2770,7 +2780,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <v>8</v>
       </c>
@@ -2790,7 +2800,7 @@
         <v>-2.89</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>9</v>
       </c>
@@ -2810,7 +2820,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
         <v>10</v>
       </c>
@@ -2830,7 +2840,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>11</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <v>12</v>
       </c>
@@ -2870,7 +2880,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>13</v>
       </c>
@@ -2890,7 +2900,7 @@
         <v>-180</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <v>14</v>
       </c>
@@ -2910,7 +2920,7 @@
         <v>-1500</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G27" s="28"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Naprawiono działanie picker Konto, pozbyto się pickera z warsty View i przeniesiono do ViewModel
</commit_message>
<xml_diff>
--- a/MauiApp1.Test/Plik_xtb_do_testow.xlsx
+++ b/MauiApp1.Test/Plik_xtb_do_testow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\Documents\Visual Studio 2022\Portfolio-Tracker\MauiApp1.Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745EC3BB-C216-443D-AF78-EAC8381A41C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1111AFDF-E15E-40B1-B236-A0DDE2209DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="3330" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{D0F3F6B9-96A1-438E-B47A-37E3DCA5E30A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{D0F3F6B9-96A1-438E-B47A-37E3DCA5E30A}"/>
   </bookViews>
   <sheets>
     <sheet name="CLOSED POSITION HISTORY" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="83">
   <si>
     <t/>
   </si>
@@ -288,6 +288,21 @@
   <si>
     <t>dywidenda pko</t>
   </si>
+  <si>
+    <t>SP500</t>
+  </si>
+  <si>
+    <t>dolar</t>
+  </si>
+  <si>
+    <t>kurs</t>
+  </si>
+  <si>
+    <t>liczba akcji</t>
+  </si>
+  <si>
+    <t>suma akcji sp500</t>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +314,7 @@
     <numFmt numFmtId="166" formatCode="[$-10809]0.0000;\(0.0000\)"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +427,15 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +454,14 @@
         <bgColor rgb="FFF3F4F4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -452,13 +480,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -553,7 +596,56 @@
     <xf numFmtId="22" fontId="14" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -563,55 +655,12 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="2" xr:uid="{39118CEE-EDEF-4B02-8910-E74BADD89802}"/>
@@ -964,12 +1013,12 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="34"/>
+      <c r="V1" s="39"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="34"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -989,12 +1038,12 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="34"/>
+      <c r="V2" s="39"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1081,24 +1130,24 @@
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="34"/>
-      <c r="W6" s="34"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
@@ -1114,24 +1163,24 @@
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="34"/>
-      <c r="W7" s="34"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
@@ -1147,24 +1196,24 @@
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="39"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
@@ -1181,34 +1230,34 @@
         <v>0</v>
       </c>
       <c r="F9" s="46"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="34"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="2:24" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1248,18 +1297,18 @@
       <c r="T10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="34"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
-      <c r="X10" s="34"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
     </row>
     <row r="11" spans="2:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="6" t="s">
         <v>0</v>
       </c>
@@ -1305,22 +1354,22 @@
       <c r="T11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="U11" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
+      <c r="U11" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="V11" s="39"/>
+      <c r="W11" s="39"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
       <c r="H12" s="6" t="s">
         <v>0</v>
       </c>
@@ -1360,11 +1409,11 @@
       <c r="T12" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="U12" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
+      <c r="U12" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="2:24" ht="22.5" x14ac:dyDescent="0.25">
@@ -1425,11 +1474,11 @@
       <c r="T13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="U13" s="53" t="s">
+      <c r="U13" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
+      <c r="V13" s="39"/>
+      <c r="W13" s="39"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="2:24" ht="31.5" x14ac:dyDescent="0.25">
@@ -1484,11 +1533,11 @@
       <c r="T14" s="15">
         <v>71.400000000000006</v>
       </c>
-      <c r="U14" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
+      <c r="U14" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="2:24" ht="31.5" x14ac:dyDescent="0.25">
@@ -1543,11 +1592,11 @@
       <c r="T15" s="21">
         <v>4.12</v>
       </c>
-      <c r="U15" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
+      <c r="U15" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="2:24" ht="31.5" x14ac:dyDescent="0.25">
@@ -1602,11 +1651,11 @@
       <c r="T16" s="22">
         <v>-0.6</v>
       </c>
-      <c r="U16" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="V16" s="49"/>
-      <c r="W16" s="49"/>
+      <c r="U16" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="2:23" ht="31.5" x14ac:dyDescent="0.25">
@@ -1661,11 +1710,11 @@
       <c r="T17" s="23">
         <v>-30</v>
       </c>
-      <c r="U17" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
+      <c r="U17" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
     </row>
     <row r="18" spans="2:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
@@ -1719,11 +1768,11 @@
       <c r="T18" s="22">
         <v>-42.87</v>
       </c>
-      <c r="U18" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
+      <c r="U18" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
     </row>
     <row r="19" spans="2:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
@@ -1774,11 +1823,11 @@
         <f>M19-L19</f>
         <v>194.24600000000004</v>
       </c>
-      <c r="U19" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
+      <c r="U19" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="V19" s="39"/>
+      <c r="W19" s="39"/>
     </row>
     <row r="20" spans="2:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
@@ -2052,15 +2101,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="U12:W12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="U8:W8"/>
     <mergeCell ref="U9:W9"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="U10:X10"/>
@@ -2071,22 +2127,15 @@
     <mergeCell ref="L9:N9"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="R9:T9"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="U7:W7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="U8:W8"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="U12:W12"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2588,18 +2637,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3074FF5-456E-48C8-B2D2-F37D01749490}">
-  <dimension ref="B12:M27"/>
+  <dimension ref="B3:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T12:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="20.28515625" customWidth="1"/>
+    <col min="9" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="34">
+        <f>G13+G14+G26+G23+G24</f>
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="34">
+        <f>G19+G20</f>
+        <v>12.309999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" s="34">
+        <f>G17+G18</f>
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
         <v>35</v>
       </c>
@@ -2618,15 +2700,17 @@
       <c r="G12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" s="54">
-        <f>G13+G14+G26+G23+G24</f>
-        <v>8500</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>1</v>
       </c>
@@ -2645,8 +2729,39 @@
       <c r="G13" s="30">
         <v>16000</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>3.9849999999999999</v>
+      </c>
+      <c r="I13">
+        <v>4700.28</v>
+      </c>
+      <c r="J13">
+        <f>G13/H13/I13</f>
+        <v>0.8542164427930875</v>
+      </c>
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
+      <c r="N13">
+        <f>SUM(J13:J26)</f>
+        <v>0.47797790468848922</v>
+      </c>
+      <c r="P13" s="56">
+        <v>3.6778</v>
+      </c>
+      <c r="Q13" s="55">
+        <v>6742.4833333333299</v>
+      </c>
+      <c r="S13">
+        <f>N13*P13*Q13</f>
+        <v>11852.659578591169</v>
+      </c>
+      <c r="T13">
+        <f>(S13-L3)/L3*100</f>
+        <v>39.443053865778452</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <v>2</v>
       </c>
@@ -2665,8 +2780,18 @@
       <c r="G14" s="29">
         <v>-6000</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>4.0046999999999997</v>
+      </c>
+      <c r="I14">
+        <v>4888.8933333333298</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J26" si="0">G14/H14/I14</f>
+        <v>-0.3064578149602375</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
         <v>3</v>
       </c>
@@ -2685,15 +2810,8 @@
       <c r="G15" s="30">
         <v>-5000</v>
       </c>
-      <c r="K15" t="s">
-        <v>76</v>
-      </c>
-      <c r="L15" s="54">
-        <f>G19+G20</f>
-        <v>12.309999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <v>4</v>
       </c>
@@ -2713,7 +2831,7 @@
         <v>-3000</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>5</v>
       </c>
@@ -2733,7 +2851,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <v>6</v>
       </c>
@@ -2752,15 +2870,8 @@
       <c r="G18" s="29">
         <v>-47.5</v>
       </c>
-      <c r="K18" t="s">
-        <v>77</v>
-      </c>
-      <c r="M18" s="54">
-        <f>G17+G18</f>
-        <v>202.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>7</v>
       </c>
@@ -2780,7 +2891,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <v>8</v>
       </c>
@@ -2800,7 +2911,7 @@
         <v>-2.89</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>9</v>
       </c>
@@ -2820,7 +2931,7 @@
         <v>6200</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
         <v>10</v>
       </c>
@@ -2840,7 +2951,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>11</v>
       </c>
@@ -2860,7 +2971,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <v>12</v>
       </c>
@@ -2880,7 +2991,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>13</v>
       </c>
@@ -2900,7 +3011,7 @@
         <v>-180</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <v>14</v>
       </c>
@@ -2919,8 +3030,18 @@
       <c r="G26" s="29">
         <v>-1500</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>4.0159000000000002</v>
+      </c>
+      <c r="I26">
+        <v>5352.7</v>
+      </c>
+      <c r="J26">
+        <f>G26/H26/I26</f>
+        <v>-6.9780723144360804E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G27" s="28"/>
     </row>
   </sheetData>

</xml_diff>